<commit_message>
Revert "change package name , delete auto"
# Please enter a commit message to explain why this merge is necessary,
# especially if it merges an updated upstream into a topic branch.
#
# Lines starting with '#' will be ignored, and an empty message aborts
# the commit.
</commit_message>
<xml_diff>
--- a/protocol/通信表.xlsx
+++ b/protocol/通信表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="1040" windowWidth="25600" windowHeight="14480"/>
+    <workbookView xWindow="9120" yWindow="0" windowWidth="25600" windowHeight="14480"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>通信类型id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t>CS.CSPasswdLoginMsg.proto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆应答</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC.SCPlayerInfoMsg.proto</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -493,7 +505,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -529,7 +541,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="27" customHeight="1"/>
+    <row r="3" spans="1:3" ht="27" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="40" spans="3:3">
       <c r="C40" s="2"/>
     </row>

</xml_diff>